<commit_message>
Fix uncompleted commit. Should start working on the pc version of this game after this commit.
</commit_message>
<xml_diff>
--- a/sheet/ExtraCardData.xlsx
+++ b/sheet/ExtraCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE7F64D-6BEB-4B86-80EC-3981C3C991BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21634050-16DA-4DF0-ACED-9EE438998B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -337,17 +337,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>离场时：如果场上有其他牌，则将本牌放在房间区任意槽位中。&lt;br&gt;
-回合结束时：玩家受到1伤害。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>持续：房间区每有1张“恶魔”牌，本牌点数加1。&lt;br&gt;
 回合结束时：玩家选1张道具牌横置。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>回合结束时：如果有相邻槽位没有《沙墙》，则从使本牌所在槽位所有其他牌点数减1，然后从额外牌堆将1张《沙墙》牌放在本牌所在槽位，这之后，将本牌移动一个没有《沙墙》牌的相邻槽位中。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>离场时：如果同区域内其他槽位有牌，则将本牌放在房间区任意槽位中并横置。&lt;br&gt;
+回合结束时：玩家受到1伤害。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1266,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1298,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1330,7 +1330,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="3" t="str">
         <f t="shared" si="0"/>

</xml_diff>